<commit_message>
Updated latest Guinea data - loc_holiday,Zone,Center.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/loc_holiday.xlsx
+++ b/mosip_master/xlsx/loc_holiday.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP\Mosip Codebase\GUINEA_Pilot\GUINEA_Pilot_Mosip-Data_WuriGuinea-1.2.0.1-B1\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3B941F-5468-4239-83FC-D4929B4BA86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1F0CDE-BB06-40AD-BB2B-7C7177053ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="27">
   <si>
     <t>lang_code</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>FÃªte de l'indÃ©pendance</t>
+  </si>
+  <si>
+    <t>Guinea day</t>
   </si>
 </sst>
 </file>
@@ -930,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1356,6 +1359,47 @@
         <v>22</v>
       </c>
     </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2000010</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45567</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="2">
+        <v>45224.547017106481</v>
+      </c>
+      <c r="J11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>